<commit_message>
Updated POM to jdk 11, minor changes to data service
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -454,6 +454,12 @@
     <t>ayushpandey07</t>
   </si>
   <si>
+    <t>Keshavendra Singh</t>
+  </si>
+  <si>
+    <t>keshavendra</t>
+  </si>
+  <si>
     <t>Namburi Ramesh</t>
   </si>
   <si>
@@ -476,6 +482,30 @@
   </si>
   <si>
     <t>kumarbanti_kuma1</t>
+  </si>
+  <si>
+    <t>Purbid Bambroo</t>
+  </si>
+  <si>
+    <t>purbid_bambroo</t>
+  </si>
+  <si>
+    <t>Ankur Singh</t>
+  </si>
+  <si>
+    <t>ankur_singh4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanmith Mallikarjun </t>
+  </si>
+  <si>
+    <t>sanmith_mallika1</t>
+  </si>
+  <si>
+    <t>Kiran S</t>
+  </si>
+  <si>
+    <t>kiran_subramoni1</t>
   </si>
 </sst>
 </file>
@@ -807,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A77" activeCellId="3" sqref="A1:XFD1 A10:XFD10 A65:XFD65 A77:XFD77"/>
+      <selection activeCell="A63" sqref="A63:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1431,6 +1461,46 @@
         <v>153</v>
       </c>
     </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated profiles with eliminations
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1017,7 +1017,7 @@
         <v>29</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1149,7 +1149,7 @@
         <v>53</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1270,7 +1270,7 @@
         <v>75</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1468,7 +1468,7 @@
         <v>111</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1490,7 +1490,7 @@
         <v>115</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">

</xml_diff>

<commit_message>
added new profile, added  college name column
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>ankit13555</t>
+  </si>
+  <si>
+    <t>Sanjib Panda</t>
+  </si>
+  <si>
+    <t>sanjib_panda</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1795,17 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C90" s="3">
+        <v>0.0</v>
+      </c>
+    </row>
     <row r="91" ht="15.75" customHeight="1"/>
     <row r="92" ht="15.75" customHeight="1"/>
     <row r="93" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Profile updates week 16
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -958,8 +958,8 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2">
-        <v>1.0</v>
+      <c r="C10" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -1750,8 +1750,8 @@
       <c r="B82" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C82" s="2">
-        <v>0.0</v>
+      <c r="C82" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -1816,8 +1816,8 @@
       <c r="B88" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="2">
-        <v>0.0</v>
+      <c r="C88" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 19 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1163,7 +1163,7 @@
         <v>55</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
@@ -1449,7 +1449,7 @@
         <v>107</v>
       </c>
       <c r="C54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" customHeight="1">
@@ -1548,7 +1548,7 @@
         <v>125</v>
       </c>
       <c r="C63" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1">
@@ -1790,7 +1790,7 @@
         <v>169</v>
       </c>
       <c r="C85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1">
@@ -1845,7 +1845,7 @@
         <v>179</v>
       </c>
       <c r="C90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 20 profile updates
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1141,7 +1141,7 @@
         <v>51</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 21 profile updates
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1460,7 +1460,7 @@
         <v>109</v>
       </c>
       <c r="C55" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 22 profile updates
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -590,13 +590,19 @@
   </si>
   <si>
     <t>padarthyharibabu</t>
+  </si>
+  <si>
+    <t>Ashutosh Menghrajani</t>
+  </si>
+  <si>
+    <t>ashu_menghrajani</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -610,6 +616,11 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -632,11 +643,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -965,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1914,22 +1926,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="97" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="99" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="102" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="103" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="104" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="105" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="106" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="107" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="108" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="109" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="110" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="111" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="112" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
     <row r="115" ht="15.75" customHeight="1"/>
@@ -2819,6 +2841,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new joiners profile
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -596,6 +596,24 @@
   </si>
   <si>
     <t>ashu_menghrajani</t>
+  </si>
+  <si>
+    <t>saboo_aparna1</t>
+  </si>
+  <si>
+    <t>Aparna Saboo</t>
+  </si>
+  <si>
+    <t>yashok42</t>
+  </si>
+  <si>
+    <t>Ashok Yadav</t>
+  </si>
+  <si>
+    <t>kanhu_panda</t>
+  </si>
+  <si>
+    <t>Kanhucharan Panda</t>
   </si>
 </sst>
 </file>
@@ -859,7 +877,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1937,9 +1955,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A98" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A99" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A100" t="s">
+        <v>199</v>
+      </c>
+      <c r="B100" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0</v>
+      </c>
+    </row>
     <row r="101" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="102" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="103" spans="1:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added a new profile
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>Kanhucharan Panda</t>
+  </si>
+  <si>
+    <t>vinayak_chiluka</t>
+  </si>
+  <si>
+    <t>Vinayak Chiluka</t>
   </si>
 </sst>
 </file>
@@ -876,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1988,7 +1994,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A101" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="102" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="103" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="104" spans="1:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Profile update - one elimination
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1111,7 +1111,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Sort based on remaining questions
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -895,7 +895,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1992,7 +1992,7 @@
         <v>196</v>
       </c>
       <c r="C99" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 28 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -895,7 +895,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2014,7 +2014,7 @@
         <v>200</v>
       </c>
       <c r="C101" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 31 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1453,7 +1453,7 @@
         <v>99</v>
       </c>
       <c r="C50" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1">
@@ -1783,7 +1783,7 @@
         <v>159</v>
       </c>
       <c r="C80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1">
@@ -1959,7 +1959,7 @@
         <v>191</v>
       </c>
       <c r="C96" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 32 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -895,7 +895,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1970,7 +1970,7 @@
         <v>193</v>
       </c>
       <c r="C97" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 36 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -926,7 +926,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2034,7 +2034,7 @@
         <v>198</v>
       </c>
       <c r="C100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" customHeight="1">
@@ -2111,7 +2111,7 @@
         <v>213</v>
       </c>
       <c r="C107" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 38 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1330,7 +1330,7 @@
         <v>71</v>
       </c>
       <c r="C36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 40 profiles update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1363,7 +1363,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
@@ -2078,7 +2078,7 @@
         <v>206</v>
       </c>
       <c r="C104" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" customHeight="1">
@@ -2100,7 +2100,7 @@
         <v>211</v>
       </c>
       <c r="C106" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" customHeight="1">
@@ -2122,7 +2122,7 @@
         <v>215</v>
       </c>
       <c r="C108" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added new joiners profiles
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -662,6 +662,24 @@
   </si>
   <si>
     <t>NimitBnsl</t>
+  </si>
+  <si>
+    <t>Prabhat Kumar</t>
+  </si>
+  <si>
+    <t>prabhat236218</t>
+  </si>
+  <si>
+    <t>raghu96</t>
+  </si>
+  <si>
+    <t>Raghu Mahajan</t>
+  </si>
+  <si>
+    <t>Hardy Tom</t>
+  </si>
+  <si>
+    <t>hardytom</t>
   </si>
 </sst>
 </file>
@@ -925,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2125,9 +2143,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="109" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A109" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A110" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B110" t="s">
+        <v>218</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A111" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" s="4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="112" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Week 43 profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -959,7 +959,7 @@
   <dimension ref="A1:C999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2100,7 +2100,7 @@
         <v>204</v>
       </c>
       <c r="C103" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 44 profile updates
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="229">
   <si>
     <t>Anirudh Balakka</t>
   </si>
@@ -695,6 +695,12 @@
   </si>
   <si>
     <t>Navin Narshetty</t>
+  </si>
+  <si>
+    <t>archit_desai</t>
+  </si>
+  <si>
+    <t>Archit Anuj Desai</t>
   </si>
 </sst>
 </file>
@@ -958,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1374,7 +1380,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
@@ -1594,7 +1600,7 @@
         <v>113</v>
       </c>
       <c r="C57" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" customHeight="1">
@@ -2224,7 +2230,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="115" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A115" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" t="s">
+        <v>227</v>
+      </c>
+      <c r="C115" s="4">
+        <v>0</v>
+      </c>
+    </row>
     <row r="116" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="117" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="118" spans="1:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Week 45 profile and questions
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2172,7 +2172,7 @@
         <v>217</v>
       </c>
       <c r="C109" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Week 47 questions and profile update
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -964,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1776,7 +1776,7 @@
         <v>145</v>
       </c>
       <c r="C73" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1">
@@ -2183,7 +2183,7 @@
         <v>218</v>
       </c>
       <c r="C110" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" customHeight="1">
@@ -2205,7 +2205,7 @@
         <v>222</v>
       </c>
       <c r="C112" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="15.75" customHeight="1">
@@ -2227,7 +2227,7 @@
         <v>225</v>
       </c>
       <c r="C114" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Fix NPE while writing to excel
</commit_message>
<xml_diff>
--- a/src/main/resources/profiles.xlsx
+++ b/src/main/resources/profiles.xlsx
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2057,7 +2057,7 @@
         <v>194</v>
       </c>
       <c r="C98" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>